<commit_message>
Project {"project-name"} is saved Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Empty Project/Main.xlsx
+++ b/DESIGN/rules/Empty Project/Main.xlsx
@@ -4,17 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView windowHeight="8190" windowWidth="19635" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
-    <sheet name="Rules" sheetId="5" r:id="rId1"/>
+    <sheet name="Rules" r:id="rId1" sheetId="5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>Datatype aaa</t>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -29,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -37,18 +52,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -62,10 +96,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -223,7 +257,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -232,13 +266,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -248,7 +282,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -257,7 +291,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -266,7 +300,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -276,12 +310,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -312,7 +346,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -331,7 +365,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -343,13 +377,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Project "Empty Project" is saved. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Empty Project/Main.xlsx
+++ b/DESIGN/rules/Empty Project/Main.xlsx
@@ -4,32 +4,96 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView windowHeight="8190" windowWidth="19635" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
-    <sheet name="Rules" sheetId="5" r:id="rId1"/>
+    <sheet name="Rules" r:id="rId1" sheetId="5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>SimpleRules BigDecimal aaa()</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color rgb="000001"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -37,18 +101,274 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -62,10 +382,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -223,7 +543,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -232,13 +552,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -248,7 +568,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -257,7 +577,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -266,7 +586,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -276,12 +596,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -312,7 +632,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -331,7 +651,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -343,13 +663,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="s" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>